<commit_message>
updated data and fit models
</commit_message>
<xml_diff>
--- a/results/pvalue_table.xlsx
+++ b/results/pvalue_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austin/git/AndroidTAEnvironment/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A43681-22EC-0840-B315-E1CF804A8423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D2A8BF-E2EE-414A-842C-E37C959CFA3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{85746B35-EAB0-E34F-8B16-5A732025EEB5}"/>
+    <workbookView xWindow="-37280" yWindow="-3140" windowWidth="37280" windowHeight="21140" xr2:uid="{85746B35-EAB0-E34F-8B16-5A732025EEB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="83">
   <si>
     <t>aliasalgo</t>
   </si>
@@ -230,68 +230,65 @@
     <t>Intercept</t>
   </si>
   <si>
-    <t> -7.44</t>
-  </si>
-  <si>
-    <t> -21.44</t>
-  </si>
-  <si>
-    <t> -3.24</t>
-  </si>
-  <si>
-    <t>0.0012*</t>
-  </si>
-  <si>
-    <t> -3.96</t>
-  </si>
-  <si>
-    <t> -8.69</t>
-  </si>
-  <si>
-    <t> -0.77</t>
-  </si>
-  <si>
-    <t> -0.41</t>
-  </si>
-  <si>
-    <t>0.0408*</t>
-  </si>
-  <si>
-    <t> -0.32</t>
-  </si>
-  <si>
-    <t>0.0021*</t>
-  </si>
-  <si>
-    <t> -6.62</t>
-  </si>
-  <si>
-    <t> -3.29</t>
-  </si>
-  <si>
-    <t>0.0010*</t>
-  </si>
-  <si>
-    <t> -2.09</t>
-  </si>
-  <si>
-    <t>0.0371*</t>
-  </si>
-  <si>
-    <t> -2.77</t>
-  </si>
-  <si>
-    <t>0.0056*</t>
-  </si>
-  <si>
-    <t> -5.79</t>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>PValue</t>
+  </si>
+  <si>
+    <t> -53.67</t>
+  </si>
+  <si>
+    <t> -30.43</t>
+  </si>
+  <si>
+    <t> -220.10</t>
+  </si>
+  <si>
+    <t> -6.99</t>
+  </si>
+  <si>
+    <t> -16.00</t>
+  </si>
+  <si>
+    <t> -22.93</t>
+  </si>
+  <si>
+    <t> -11.19</t>
+  </si>
+  <si>
+    <t> -8.61</t>
+  </si>
+  <si>
+    <t> -8.85</t>
+  </si>
+  <si>
+    <t>0.0262*</t>
+  </si>
+  <si>
+    <t>0.0003*</t>
+  </si>
+  <si>
+    <t> -8.49</t>
+  </si>
+  <si>
+    <t> -31.79</t>
+  </si>
+  <si>
+    <t> -21.65</t>
+  </si>
+  <si>
+    <t> -25.17</t>
+  </si>
+  <si>
+    <t> -27.30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -366,8 +363,22 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,8 +397,13 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -490,11 +506,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -524,7 +565,13 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,19 +587,158 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -594,7 +780,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="13"/>
         <color theme="0"/>
         <name val="Helvetica"/>
         <family val="2"/>
@@ -606,6 +792,22 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -676,40 +878,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -727,60 +895,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -790,12 +904,18 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
+        <sz val="12"/>
+        <color theme="0"/>
         <name val="Helvetica"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -811,32 +931,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C8894D6-2576-F54C-987B-0B2D6816592A}" name="Table1" displayName="Table1" ref="U1:V44" totalsRowShown="0" headerRowDxfId="11" dataDxfId="8">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="U2:V44">
-    <sortCondition ref="U4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{21DA05DF-9AAB-EC40-8A3E-3209C9C0CBEB}" name="Table3" displayName="Table3" ref="Y1:AA24" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="Y1:AA24" xr:uid="{33E01F4E-1EE5-E04E-B57B-780E04FAC794}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y2:AA24">
+    <sortCondition ref="Y1:Y24"/>
   </sortState>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{063E2F51-5D58-B54F-827B-DFCE455C1094}" name="Term" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{1BB83A5D-DF81-3442-B90B-3C2E03D3C1E9}" name="Estimate" dataDxfId="9"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{EF0AAB32-9E63-FC40-B3B8-1C05A673B8A1}" name="Term" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{F87234D8-3B97-5D46-918D-C22CF38345A3}" name="Estimate" dataDxfId="11">
+      <calculatedColumnFormula>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{F592794F-12A5-E94A-97BE-193D9300BECE}" name="rank" dataDxfId="10">
+      <calculatedColumnFormula>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{21DA05DF-9AAB-EC40-8A3E-3209C9C0CBEB}" name="Table3" displayName="Table3" ref="Y1:AA24" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="7">
-  <autoFilter ref="Y1:AA24" xr:uid="{33E01F4E-1EE5-E04E-B57B-780E04FAC794}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y2:AA24">
-    <sortCondition ref="Y1:Y24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60A63969-E6D9-A844-B8B8-D87D44289D52}" name="Table1" displayName="Table1" ref="U1:V26" totalsRowShown="0" headerRowDxfId="8" dataDxfId="1" tableBorderDxfId="9">
+  <autoFilter ref="U1:V26" xr:uid="{36D10555-0186-7549-9AC5-0986B6AC17D2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="U2:V26">
+    <sortCondition ref="U1:U26"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EF0AAB32-9E63-FC40-B3B8-1C05A673B8A1}" name="Term" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F87234D8-3B97-5D46-918D-C22CF38345A3}" name="Estimate" dataDxfId="5">
-      <calculatedColumnFormula>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{F592794F-12A5-E94A-97BE-193D9300BECE}" name="rank" dataDxfId="4">
-      <calculatedColumnFormula>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</calculatedColumnFormula>
-    </tableColumn>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6A78A226-1B56-8640-9DBC-8C03236F24E0}" name="Term" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{538CC6A7-613B-2B45-A448-015C7FBC6B75}" name="Estimate" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1139,124 +1260,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3DAE27-83F2-0A40-93C3-548CDFD4E9EE}">
-  <dimension ref="A1:AA53"/>
+  <dimension ref="A1:AA52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D5" sqref="D5:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="27.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="25" width="10.83203125" style="1"/>
-    <col min="26" max="26" width="12" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="21" width="10.83203125" style="1"/>
+    <col min="22" max="22" width="11.6640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11" style="1" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="1"/>
+    <col min="25" max="25" width="12" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="M1" s="31" t="s">
+      <c r="K1" s="33"/>
+      <c r="M1" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31" t="s">
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31" t="s">
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="V1" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="Y1" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="Z1" s="38" t="s">
+      <c r="Z1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="AA1" s="38" t="s">
+      <c r="AA1" s="31" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="17">
       <c r="A2" s="8"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="M2" s="32" t="s">
+      <c r="K2" s="36"/>
+      <c r="M2" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="32">
-        <v>3206751.2401999999</v>
-      </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32">
-        <v>36487.08</v>
-      </c>
-      <c r="Q2" s="32">
-        <v>87.89</v>
-      </c>
-      <c r="R2" s="33" t="s">
+      <c r="N2" s="26">
+        <v>96202537.206</v>
+      </c>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26">
+        <v>45735.4</v>
+      </c>
+      <c r="Q2" s="26">
+        <v>1912.47</v>
+      </c>
+      <c r="R2" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="32" t="s">
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="32">
-        <v>348845.28016000002</v>
-      </c>
-      <c r="Y2" s="37" t="s">
+      <c r="V2" s="26">
+        <v>10465358.404999999</v>
+      </c>
+      <c r="Y2" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>348845.28016000002</v>
-      </c>
-      <c r="AA2" s="35">
+      <c r="Z2" s="26">
+        <v>10465358.404999999</v>
+      </c>
+      <c r="AA2" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>5</v>
       </c>
@@ -1293,38 +1416,38 @@
       <c r="K3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="32">
-        <v>392600.22447999998</v>
-      </c>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32">
-        <v>76816.44</v>
-      </c>
-      <c r="Q3" s="32">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="R3" s="33" t="s">
+      <c r="N3" s="26">
+        <v>11778006.733999999</v>
+      </c>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26">
+        <v>96286.96</v>
+      </c>
+      <c r="Q3" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="32" t="s">
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="32">
-        <v>392600.22447999998</v>
-      </c>
-      <c r="Y3" s="36" t="s">
+      <c r="V3" s="26">
+        <v>11778006.733999999</v>
+      </c>
+      <c r="Y3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="Z3" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>392600.22447999998</v>
-      </c>
-      <c r="AA3" s="35">
+      <c r="Z3" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>11778006.733999999</v>
+      </c>
+      <c r="AA3" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>4</v>
       </c>
@@ -1335,38 +1458,38 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="5"/>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="32">
-        <v>471542.57741000003</v>
-      </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32">
-        <v>63417.04</v>
-      </c>
-      <c r="Q4" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="R4" s="33" t="s">
+      <c r="N4" s="26">
+        <v>14146277.322000001</v>
+      </c>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26">
+        <v>79491.240000000005</v>
+      </c>
+      <c r="Q4" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32" t="s">
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="V4" s="32">
-        <v>193835.27179</v>
-      </c>
-      <c r="Y4" s="36" t="s">
+      <c r="V4" s="26">
+        <v>5815058.1538000004</v>
+      </c>
+      <c r="Y4" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="Z4" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>193835.27179</v>
-      </c>
-      <c r="AA4" s="35">
+      <c r="Z4" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>5815058.1538000004</v>
+      </c>
+      <c r="AA4" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>10</v>
       </c>
@@ -1375,23 +1498,23 @@
       <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="40">
         <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="40">
         <v>0</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" s="19">
-        <v>8.5999999999999998E-4</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>55</v>
@@ -1405,38 +1528,38 @@
       <c r="K5" s="5">
         <v>3</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="N5" s="32">
-        <v>1109382.7172000001</v>
-      </c>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32">
-        <v>65204.46</v>
-      </c>
-      <c r="Q5" s="32">
-        <v>17.010000000000002</v>
-      </c>
-      <c r="R5" s="33" t="s">
+      <c r="N5" s="26">
+        <v>33281481.515999999</v>
+      </c>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26">
+        <v>81731.710000000006</v>
+      </c>
+      <c r="Q5" s="26">
+        <v>109.22</v>
+      </c>
+      <c r="R5" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32" t="s">
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="V5" s="32">
-        <v>168401.31758999999</v>
-      </c>
-      <c r="Y5" s="37" t="s">
+      <c r="V5" s="26">
+        <v>5052039.5275999997</v>
+      </c>
+      <c r="Y5" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="Z5" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>168401.31758999999</v>
-      </c>
-      <c r="AA5" s="35">
+      <c r="Z5" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>5052039.5275999997</v>
+      </c>
+      <c r="AA5" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>11</v>
       </c>
@@ -1445,20 +1568,20 @@
       <c r="A6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="40">
         <v>0</v>
       </c>
       <c r="C6" s="1">
         <v>14</v>
       </c>
-      <c r="D6" s="19">
-        <v>1.6000000000000001E-3</v>
+      <c r="D6" s="40">
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>15</v>
       </c>
       <c r="F6" s="19">
-        <v>0.56398000000000004</v>
+        <v>3.3E-3</v>
       </c>
       <c r="G6" s="1">
         <v>20</v>
@@ -1475,38 +1598,38 @@
       <c r="K6" s="5">
         <v>18</v>
       </c>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="32">
-        <v>1627964.6825999999</v>
-      </c>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32">
-        <v>75928.149999999994</v>
-      </c>
-      <c r="Q6" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="R6" s="33" t="s">
+      <c r="N6" s="26">
+        <v>48838940.479000002</v>
+      </c>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26">
+        <v>95173.52</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="32" t="s">
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="V6" s="32">
-        <v>41270.199702999998</v>
-      </c>
-      <c r="Y6" s="36" t="s">
+      <c r="V6" s="26">
+        <v>1238105.9911</v>
+      </c>
+      <c r="Y6" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="Z6" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>41270.199702999998</v>
-      </c>
-      <c r="AA6" s="35">
+      <c r="Z6" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>1238105.9911</v>
+      </c>
+      <c r="AA6" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>19</v>
       </c>
@@ -1515,23 +1638,23 @@
       <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="19">
-        <v>0.69849000000000006</v>
+      <c r="B7" s="40">
+        <v>4.5159999999999999E-2</v>
       </c>
       <c r="C7" s="1">
         <v>22</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="40">
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="19">
-        <v>0.15611</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>55</v>
@@ -1545,38 +1668,38 @@
       <c r="K7" s="5">
         <v>10</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="N7" s="32">
-        <v>518581.96542999998</v>
-      </c>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32">
-        <v>61780.74</v>
-      </c>
-      <c r="Q7" s="32">
-        <v>8.39</v>
-      </c>
-      <c r="R7" s="33" t="s">
+      <c r="N7" s="26">
+        <v>15557458.963</v>
+      </c>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26">
+        <v>77440.19</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>155.22999999999999</v>
+      </c>
+      <c r="R7" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32" t="s">
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="V7" s="32">
-        <v>81743.819359000001</v>
-      </c>
-      <c r="Y7" s="37" t="s">
+      <c r="V7" s="26">
+        <v>2452314.5808000001</v>
+      </c>
+      <c r="Y7" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="Z7" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>81743.819359000001</v>
-      </c>
-      <c r="AA7" s="35">
+      <c r="Z7" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>2452314.5808000001</v>
+      </c>
+      <c r="AA7" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>17</v>
       </c>
@@ -1585,20 +1708,20 @@
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19">
-        <v>1.3799999999999999E-3</v>
+      <c r="B8" s="40">
+        <v>0</v>
       </c>
       <c r="C8" s="1">
         <v>15</v>
       </c>
-      <c r="D8" s="19">
-        <v>0.1404</v>
+      <c r="D8" s="40">
+        <v>0</v>
       </c>
       <c r="E8" s="1">
         <v>16</v>
       </c>
       <c r="F8" s="19">
-        <v>9.0649999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
         <v>16</v>
@@ -1610,43 +1733,43 @@
         <v>55</v>
       </c>
       <c r="J8" s="22">
-        <v>0.58723999999999998</v>
+        <v>0.15171000000000001</v>
       </c>
       <c r="K8" s="5">
         <v>22</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="M8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="32">
-        <v>348845.28016000002</v>
-      </c>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32">
-        <v>54012.45</v>
-      </c>
-      <c r="Q8" s="32">
-        <v>6.46</v>
-      </c>
-      <c r="R8" s="33" t="s">
+      <c r="N8" s="26">
+        <v>10465358.404999999</v>
+      </c>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26">
+        <v>67702.880000000005</v>
+      </c>
+      <c r="Q8" s="26">
+        <v>9.19</v>
+      </c>
+      <c r="R8" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S8" s="33"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="32" t="s">
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="V8" s="32">
-        <v>210920.08975000001</v>
-      </c>
-      <c r="Y8" s="36" t="s">
+      <c r="V8" s="26">
+        <v>6327602.6924999999</v>
+      </c>
+      <c r="Y8" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="Z8" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>210920.08975000001</v>
-      </c>
-      <c r="AA8" s="35">
+      <c r="Z8" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>6327602.6924999999</v>
+      </c>
+      <c r="AA8" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>9</v>
       </c>
@@ -1655,23 +1778,23 @@
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="19">
-        <v>1.4400000000000001E-3</v>
+      <c r="B9" s="40">
+        <v>0</v>
       </c>
       <c r="C9" s="1">
         <v>18</v>
       </c>
-      <c r="D9" s="19">
-        <v>0.81996000000000002</v>
+      <c r="D9" s="40">
+        <v>0</v>
       </c>
       <c r="E9" s="1">
         <v>22</v>
       </c>
       <c r="F9" s="19">
-        <v>1.4400000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>55</v>
@@ -1685,38 +1808,38 @@
       <c r="K9" s="5">
         <v>14</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="32">
-        <v>193835.27179</v>
-      </c>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32">
-        <v>49492.35</v>
-      </c>
-      <c r="Q9" s="32">
-        <v>3.92</v>
-      </c>
-      <c r="R9" s="33" t="s">
+      <c r="N9" s="26">
+        <v>5815058.1538000004</v>
+      </c>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26">
+        <v>62037.09</v>
+      </c>
+      <c r="Q9" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="R9" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S9" s="33"/>
-      <c r="T9" s="33"/>
-      <c r="U9" s="32" t="s">
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="V9" s="32">
-        <v>471542.57741000003</v>
-      </c>
-      <c r="Y9" s="37" t="s">
+      <c r="V9" s="26">
+        <v>14146277.322000001</v>
+      </c>
+      <c r="Y9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="Z9" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>471542.57741000003</v>
-      </c>
-      <c r="AA9" s="35">
+      <c r="Z9" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>14146277.322000001</v>
+      </c>
+      <c r="AA9" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>3</v>
       </c>
@@ -1725,23 +1848,23 @@
       <c r="A10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="40">
         <v>0</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="40">
         <v>0</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="19">
-        <v>7.3999999999999999E-4</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>55</v>
@@ -1755,38 +1878,38 @@
       <c r="K10" s="5">
         <v>2</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="M10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="32">
-        <v>168401.31758999999</v>
-      </c>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32">
-        <v>51937.31</v>
-      </c>
-      <c r="Q10" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="R10" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="S10" s="33"/>
-      <c r="T10" s="33"/>
-      <c r="U10" s="32" t="s">
+      <c r="N10" s="26">
+        <v>5052039.5275999997</v>
+      </c>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26">
+        <v>65101.760000000002</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>20.56</v>
+      </c>
+      <c r="R10" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="V10" s="32">
-        <v>478469.54096999997</v>
-      </c>
-      <c r="Y10" s="37" t="s">
+      <c r="V10" s="26">
+        <v>14354086.229</v>
+      </c>
+      <c r="Y10" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="Z10" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>478469.54096999997</v>
-      </c>
-      <c r="AA10" s="35">
+      <c r="Z10" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>14354086.229</v>
+      </c>
+      <c r="AA10" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>2</v>
       </c>
@@ -1795,23 +1918,23 @@
       <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="40">
         <v>0</v>
       </c>
       <c r="C11" s="1">
         <v>13</v>
       </c>
-      <c r="D11" s="19">
-        <v>1.2600000000000001E-3</v>
+      <c r="D11" s="40">
+        <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F11" s="19">
-        <v>1.49E-3</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>55</v>
@@ -1825,38 +1948,38 @@
       <c r="K11" s="5">
         <v>7</v>
       </c>
-      <c r="M11" s="32" t="s">
+      <c r="M11" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="N11" s="32">
-        <v>41270.199702999998</v>
-      </c>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32">
-        <v>54324.44</v>
-      </c>
-      <c r="Q11" s="32">
-        <v>0.76</v>
-      </c>
-      <c r="R11" s="32">
-        <v>0.44750000000000001</v>
-      </c>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="32" t="s">
+      <c r="N11" s="26">
+        <v>1238105.9911</v>
+      </c>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26">
+        <v>68093.95</v>
+      </c>
+      <c r="Q11" s="26">
+        <v>17.79</v>
+      </c>
+      <c r="R11" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="V11" s="32">
-        <v>37878.973962999997</v>
-      </c>
-      <c r="Y11" s="36" t="s">
+      <c r="V11" s="26">
+        <v>1136369.2189</v>
+      </c>
+      <c r="Y11" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="Z11" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>37878.973962999997</v>
-      </c>
-      <c r="AA11" s="35">
+      <c r="Z11" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>1136369.2189</v>
+      </c>
+      <c r="AA11" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>20</v>
       </c>
@@ -1865,20 +1988,20 @@
       <c r="A12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="40">
         <v>0</v>
       </c>
       <c r="C12" s="1">
         <v>7</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="40">
         <v>0</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
       </c>
       <c r="F12" s="19">
-        <v>0.40625</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="G12" s="1">
         <v>19</v>
@@ -1895,38 +2018,38 @@
       <c r="K12" s="5">
         <v>16</v>
       </c>
-      <c r="M12" s="32" t="s">
+      <c r="M12" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="N12" s="32">
-        <v>81743.819359000001</v>
-      </c>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32">
-        <v>51230.18</v>
-      </c>
-      <c r="Q12" s="32">
-        <v>1.6</v>
-      </c>
-      <c r="R12" s="32">
-        <v>0.1106</v>
-      </c>
-      <c r="S12" s="34"/>
-      <c r="T12" s="34"/>
-      <c r="U12" s="32" t="s">
+      <c r="N12" s="26">
+        <v>2452314.5808000001</v>
+      </c>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26">
+        <v>64215.4</v>
+      </c>
+      <c r="Q12" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="R12" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="V12" s="32">
-        <v>18704.295756</v>
-      </c>
-      <c r="Y12" s="37" t="s">
+      <c r="V12" s="26">
+        <v>561128.87268999999</v>
+      </c>
+      <c r="Y12" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="Z12" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>18704.295756</v>
-      </c>
-      <c r="AA12" s="35">
+      <c r="Z12" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>561128.87268999999</v>
+      </c>
+      <c r="AA12" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>22</v>
       </c>
@@ -1935,23 +2058,23 @@
       <c r="A13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="19">
-        <v>6.7600000000000004E-3</v>
+      <c r="B13" s="40">
+        <v>0</v>
       </c>
       <c r="C13" s="1">
         <v>19</v>
       </c>
-      <c r="D13" s="19">
-        <v>1.6000000000000001E-4</v>
+      <c r="D13" s="40">
+        <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="19">
-        <v>7.5000000000000002E-4</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>55</v>
@@ -1960,43 +2083,43 @@
         <v>55</v>
       </c>
       <c r="J13" s="22">
-        <v>2.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="K13" s="5">
         <v>20</v>
       </c>
-      <c r="M13" s="32" t="s">
+      <c r="M13" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="N13" s="32">
-        <v>210920.08975000001</v>
-      </c>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32">
-        <v>53230.81</v>
-      </c>
-      <c r="Q13" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="R13" s="33" t="s">
+      <c r="N13" s="26">
+        <v>6327602.6924999999</v>
+      </c>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26">
+        <v>66723.12</v>
+      </c>
+      <c r="Q13" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="R13" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32" t="s">
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="V13" s="32">
-        <v>136715.68515999999</v>
-      </c>
-      <c r="Y13" s="36" t="s">
+      <c r="V13" s="26">
+        <v>4101470.5548</v>
+      </c>
+      <c r="Y13" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>136715.68515999999</v>
-      </c>
-      <c r="AA13" s="35">
+      <c r="Z13" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>4101470.5548</v>
+      </c>
+      <c r="AA13" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>15</v>
       </c>
@@ -2005,23 +2128,23 @@
       <c r="A14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="40">
         <v>0</v>
       </c>
       <c r="C14" s="1">
         <v>10</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="40">
         <v>0</v>
       </c>
       <c r="E14" s="1">
         <v>4</v>
       </c>
       <c r="F14" s="19">
-        <v>2.97E-3</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>55</v>
@@ -2035,38 +2158,38 @@
       <c r="K14" s="5">
         <v>6</v>
       </c>
-      <c r="M14" s="32" t="s">
+      <c r="M14" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="N14" s="32">
-        <v>478469.54096999997</v>
-      </c>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32">
-        <v>55069.05</v>
-      </c>
-      <c r="Q14" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="R14" s="33" t="s">
+      <c r="N14" s="26">
+        <v>14354086.229</v>
+      </c>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26">
+        <v>69027.3</v>
+      </c>
+      <c r="Q14" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="R14" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S14" s="32"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="32" t="s">
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="V14" s="32">
-        <v>16742.738526000001</v>
-      </c>
-      <c r="Y14" s="37" t="s">
+      <c r="V14" s="26">
+        <v>502282.15577999997</v>
+      </c>
+      <c r="Y14" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="Z14" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>16742.738526000001</v>
-      </c>
-      <c r="AA14" s="35">
+      <c r="Z14" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>502282.15577999997</v>
+      </c>
+      <c r="AA14" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>23</v>
       </c>
@@ -2075,23 +2198,23 @@
       <c r="A15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="40">
         <v>0</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
       </c>
-      <c r="D15" s="19">
-        <v>4.3899999999999998E-3</v>
+      <c r="D15" s="40">
+        <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15" s="19">
-        <v>1.6199999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>55</v>
@@ -2105,38 +2228,38 @@
       <c r="K15" s="5">
         <v>5</v>
       </c>
-      <c r="M15" s="32" t="s">
+      <c r="M15" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="32">
-        <v>37878.973962999997</v>
-      </c>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32">
-        <v>49239.48</v>
-      </c>
-      <c r="Q15" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="R15" s="32">
-        <v>0.44180000000000003</v>
-      </c>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
-      <c r="U15" s="32" t="s">
+      <c r="N15" s="26">
+        <v>1136369.2189</v>
+      </c>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26">
+        <v>61720.12</v>
+      </c>
+      <c r="Q15" s="26">
+        <v>15.63</v>
+      </c>
+      <c r="R15" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="V15" s="32">
-        <v>162923.89726</v>
-      </c>
-      <c r="Y15" s="36" t="s">
+      <c r="V15" s="26">
+        <v>4887716.9178999998</v>
+      </c>
+      <c r="Y15" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="Z15" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>162923.89726</v>
-      </c>
-      <c r="AA15" s="35">
+      <c r="Z15" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>4887716.9178999998</v>
+      </c>
+      <c r="AA15" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>13</v>
       </c>
@@ -2145,23 +2268,23 @@
       <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="40">
         <v>0</v>
       </c>
       <c r="C16" s="1">
         <v>9</v>
       </c>
-      <c r="D16" s="19">
-        <v>0.45408999999999999</v>
+      <c r="D16" s="40">
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F16" s="19">
-        <v>0.33912999999999999</v>
+        <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>55</v>
@@ -2175,38 +2298,38 @@
       <c r="K16" s="5">
         <v>11</v>
       </c>
-      <c r="M16" s="32" t="s">
+      <c r="M16" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="32">
-        <v>18704.295756</v>
-      </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32">
-        <v>45628.23</v>
-      </c>
-      <c r="Q16" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="R16" s="32">
-        <v>0.68189999999999995</v>
-      </c>
-      <c r="S16" s="34"/>
-      <c r="T16" s="34"/>
-      <c r="U16" s="32" t="s">
+      <c r="N16" s="26">
+        <v>561128.87268999999</v>
+      </c>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26">
+        <v>57193.53</v>
+      </c>
+      <c r="Q16" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="R16" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="V16" s="32">
-        <v>36129.166923999997</v>
-      </c>
-      <c r="Y16" s="37" t="s">
+      <c r="V16" s="26">
+        <v>1083875.0077</v>
+      </c>
+      <c r="Y16" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="Z16" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>36129.166923999997</v>
-      </c>
-      <c r="AA16" s="35">
+      <c r="Z16" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>1083875.0077</v>
+      </c>
+      <c r="AA16" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>21</v>
       </c>
@@ -2215,13 +2338,13 @@
       <c r="A17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="40">
         <v>0</v>
       </c>
       <c r="C17" s="1">
         <v>8</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="40">
         <v>0</v>
       </c>
       <c r="E17" s="1">
@@ -2231,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>55</v>
@@ -2245,38 +2368,38 @@
       <c r="K17" s="5">
         <v>17</v>
       </c>
-      <c r="M17" s="32" t="s">
+      <c r="M17" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="N17" s="32">
-        <v>136715.68515999999</v>
-      </c>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32">
-        <v>66806.83</v>
-      </c>
-      <c r="Q17" s="32">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="R17" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="S17" s="32"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="32" t="s">
+      <c r="N17" s="26">
+        <v>4101470.5548</v>
+      </c>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26">
+        <v>83740.23</v>
+      </c>
+      <c r="Q17" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="R17" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="V17" s="32">
-        <v>78352.181058000002</v>
-      </c>
-      <c r="Y17" s="36" t="s">
+      <c r="V17" s="26">
+        <v>2350565.4317999999</v>
+      </c>
+      <c r="Y17" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="Z17" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>78352.181058000002</v>
-      </c>
-      <c r="AA17" s="35">
+      <c r="Z17" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>2350565.4317999999</v>
+      </c>
+      <c r="AA17" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>18</v>
       </c>
@@ -2285,20 +2408,20 @@
       <c r="A18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="40">
         <v>0</v>
       </c>
       <c r="C18" s="1">
         <v>12</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="40">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F18" s="19">
-        <v>0.69360999999999995</v>
+        <v>4.4769999999999997E-2</v>
       </c>
       <c r="G18" s="1">
         <v>21</v>
@@ -2310,43 +2433,43 @@
         <v>55</v>
       </c>
       <c r="J18" s="22">
-        <v>2.351E-2</v>
+        <v>0</v>
       </c>
       <c r="K18" s="5">
         <v>21</v>
       </c>
-      <c r="M18" s="32" t="s">
+      <c r="M18" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="N18" s="32">
-        <v>16742.738526000001</v>
-      </c>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32">
-        <v>52890.080000000002</v>
-      </c>
-      <c r="Q18" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="R18" s="32">
-        <v>0.75160000000000005</v>
-      </c>
-      <c r="S18" s="33"/>
-      <c r="T18" s="33"/>
-      <c r="U18" s="32" t="s">
+      <c r="N18" s="26">
+        <v>502282.15577999997</v>
+      </c>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26">
+        <v>66296.03</v>
+      </c>
+      <c r="Q18" s="26">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="R18" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="V18" s="32">
-        <v>307876.74385000003</v>
-      </c>
-      <c r="Y18" s="37" t="s">
+      <c r="V18" s="26">
+        <v>9236302.3155000005</v>
+      </c>
+      <c r="Y18" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="Z18" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>307876.74385000003</v>
-      </c>
-      <c r="AA18" s="35">
+      <c r="Z18" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>9236302.3155000005</v>
+      </c>
+      <c r="AA18" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>7</v>
       </c>
@@ -2355,23 +2478,23 @@
       <c r="A19" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="19">
-        <v>0.14544000000000001</v>
+      <c r="B19" s="40">
+        <v>0</v>
       </c>
       <c r="C19" s="1">
         <v>21</v>
       </c>
-      <c r="D19" s="19">
-        <v>0.12107</v>
+      <c r="D19" s="40">
+        <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="19">
-        <v>1.031E-2</v>
+        <v>0</v>
       </c>
       <c r="G19" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>55</v>
@@ -2385,38 +2508,38 @@
       <c r="K19" s="5">
         <v>13</v>
       </c>
-      <c r="M19" s="32" t="s">
+      <c r="M19" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="N19" s="32">
-        <v>162923.89726</v>
-      </c>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32">
-        <v>52929.71</v>
-      </c>
-      <c r="Q19" s="32">
-        <v>3.08</v>
-      </c>
-      <c r="R19" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32" t="s">
+      <c r="N19" s="26">
+        <v>4887716.9178999998</v>
+      </c>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26">
+        <v>66345.7</v>
+      </c>
+      <c r="Q19" s="26">
+        <v>3.58</v>
+      </c>
+      <c r="R19" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="V19" s="32">
-        <v>165769.11780000001</v>
-      </c>
-      <c r="Y19" s="36" t="s">
+      <c r="V19" s="26">
+        <v>4973073.5339000002</v>
+      </c>
+      <c r="Y19" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="Z19" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>165769.11780000001</v>
-      </c>
-      <c r="AA19" s="35">
+      <c r="Z19" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>4973073.5339000002</v>
+      </c>
+      <c r="AA19" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>12</v>
       </c>
@@ -2425,13 +2548,13 @@
       <c r="A20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="19">
-        <v>4.6999999999999999E-4</v>
+      <c r="B20" s="40">
+        <v>0</v>
       </c>
       <c r="C20" s="1">
         <v>17</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="40">
         <v>0</v>
       </c>
       <c r="E20" s="1">
@@ -2441,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>55</v>
@@ -2455,38 +2578,38 @@
       <c r="K20" s="5">
         <v>1</v>
       </c>
-      <c r="M20" s="32" t="s">
+      <c r="M20" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="N20" s="32">
-        <v>36129.166923999997</v>
-      </c>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32">
-        <v>53500.49</v>
-      </c>
-      <c r="Q20" s="32">
-        <v>0.68</v>
-      </c>
-      <c r="R20" s="32">
-        <v>0.4995</v>
-      </c>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32" t="s">
+      <c r="N20" s="26">
+        <v>1083875.0077</v>
+      </c>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26">
+        <v>67061.16</v>
+      </c>
+      <c r="Q20" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="R20" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="V20" s="32">
-        <v>118294.70535</v>
-      </c>
-      <c r="Y20" s="37" t="s">
+      <c r="V20" s="26">
+        <v>3548841.1606000001</v>
+      </c>
+      <c r="Y20" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="Z20" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>118294.70535</v>
-      </c>
-      <c r="AA20" s="35">
+      <c r="Z20" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>3548841.1606000001</v>
+      </c>
+      <c r="AA20" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>16</v>
       </c>
@@ -2495,17 +2618,17 @@
       <c r="A21" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="40">
         <v>0</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
-      <c r="D21" s="19">
-        <v>0.21478</v>
+      <c r="D21" s="40">
+        <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="19">
         <v>0</v>
@@ -2525,38 +2648,38 @@
       <c r="K21" s="5">
         <v>4</v>
       </c>
-      <c r="M21" s="32" t="s">
+      <c r="M21" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="N21" s="32">
-        <v>78352.181058000002</v>
-      </c>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32">
-        <v>52326.96</v>
-      </c>
-      <c r="Q21" s="32">
-        <v>1.5</v>
-      </c>
-      <c r="R21" s="32">
-        <v>0.1343</v>
-      </c>
-      <c r="S21" s="32"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="32" t="s">
+      <c r="N21" s="26">
+        <v>2350565.4317999999</v>
+      </c>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26">
+        <v>65590.17</v>
+      </c>
+      <c r="Q21" s="26">
+        <v>10.41</v>
+      </c>
+      <c r="R21" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="V21" s="32">
-        <v>154303.99083</v>
-      </c>
-      <c r="Y21" s="36" t="s">
+      <c r="V21" s="26">
+        <v>4629119.7248999998</v>
+      </c>
+      <c r="Y21" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="Z21" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>154303.99083</v>
-      </c>
-      <c r="AA21" s="35">
+      <c r="Z21" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>4629119.7248999998</v>
+      </c>
+      <c r="AA21" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>14</v>
       </c>
@@ -2565,23 +2688,23 @@
       <c r="A22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="40">
         <v>0</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="40">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F22" s="19">
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>55</v>
@@ -2590,43 +2713,43 @@
         <v>55</v>
       </c>
       <c r="J22" s="22">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="K22" s="5">
         <v>15</v>
       </c>
-      <c r="M22" s="32" t="s">
+      <c r="M22" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="N22" s="32">
-        <v>307876.74385000003</v>
-      </c>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32">
-        <v>46472.72</v>
-      </c>
-      <c r="Q22" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="R22" s="33" t="s">
+      <c r="N22" s="26">
+        <v>9236302.3155000005</v>
+      </c>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26">
+        <v>58252.08</v>
+      </c>
+      <c r="Q22" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="R22" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="32" t="s">
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="V22" s="32">
-        <v>518581.96542999998</v>
-      </c>
-      <c r="Y22" s="36" t="s">
+      <c r="V22" s="26">
+        <v>15557458.963</v>
+      </c>
+      <c r="Y22" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="Z22" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>1627964.6825999999</v>
-      </c>
-      <c r="AA22" s="35">
+      <c r="Z22" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>48838940.479000002</v>
+      </c>
+      <c r="AA22" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>1</v>
       </c>
@@ -2635,23 +2758,23 @@
       <c r="A23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="19">
-        <v>3.2719999999999999E-2</v>
+      <c r="B23" s="40">
+        <v>0</v>
       </c>
       <c r="C23" s="1">
         <v>20</v>
       </c>
-      <c r="D23" s="19">
-        <v>0.25814999999999999</v>
+      <c r="D23" s="40">
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" s="19">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>55</v>
@@ -2665,38 +2788,38 @@
       <c r="K23" s="5">
         <v>12</v>
       </c>
-      <c r="M23" s="32" t="s">
+      <c r="M23" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="N23" s="32">
-        <v>165769.11780000001</v>
-      </c>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32">
-        <v>50403.42</v>
-      </c>
-      <c r="Q23" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="R23" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="S23" s="32"/>
-      <c r="T23" s="32"/>
-      <c r="U23" s="32" t="s">
+      <c r="N23" s="26">
+        <v>4973073.5339000002</v>
+      </c>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26">
+        <v>63179.07</v>
+      </c>
+      <c r="Q23" s="26">
+        <v>12.07</v>
+      </c>
+      <c r="R23" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="V23" s="32">
-        <v>1109382.7172000001</v>
-      </c>
-      <c r="Y23" s="37" t="s">
+      <c r="V23" s="26">
+        <v>33281481.515999999</v>
+      </c>
+      <c r="Y23" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="Z23" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>325052.75475999998</v>
-      </c>
-      <c r="AA23" s="35">
+      <c r="Z23" s="43">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>9751582.6428999994</v>
+      </c>
+      <c r="AA23" s="29">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>6</v>
       </c>
@@ -2705,20 +2828,20 @@
       <c r="A24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="19">
-        <v>1.0000000000000001E-5</v>
+      <c r="B24" s="40">
+        <v>0</v>
       </c>
       <c r="C24" s="1">
         <v>16</v>
       </c>
-      <c r="D24" s="19">
-        <v>4.1799999999999997E-2</v>
+      <c r="D24" s="40">
+        <v>0</v>
       </c>
       <c r="E24" s="1">
         <v>17</v>
       </c>
       <c r="F24" s="19">
-        <v>0.74073999999999995</v>
+        <v>9.1899999999999996E-2</v>
       </c>
       <c r="G24" s="1">
         <v>22</v>
@@ -2735,38 +2858,38 @@
       <c r="K24" s="5">
         <v>8</v>
       </c>
-      <c r="M24" s="32" t="s">
+      <c r="M24" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="N24" s="32">
-        <v>118294.70535</v>
-      </c>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32">
-        <v>56729.23</v>
-      </c>
-      <c r="Q24" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="R24" s="34" t="s">
+      <c r="N24" s="26">
+        <v>3548841.1606000001</v>
+      </c>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26">
+        <v>71108.28</v>
+      </c>
+      <c r="Q24" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="S24" s="32"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32" t="s">
+      <c r="R24" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="V24" s="32">
-        <v>1627964.6825999999</v>
-      </c>
-      <c r="Y24" s="36" t="s">
+      <c r="V24" s="26">
+        <v>48838940.479000002</v>
+      </c>
+      <c r="Y24" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="Z24" s="35">
-        <f>VLOOKUP(Table3[[#This Row],[Term]],Table1[#All],2)</f>
-        <v>299782.36228</v>
-      </c>
-      <c r="AA24" s="35">
+      <c r="Z24" s="44">
+        <f>VLOOKUP(Table3[[#This Row],[Term]],Sheet1!$U$1:$V$26,2)</f>
+        <v>8993470.8683000002</v>
+      </c>
+      <c r="AA24" s="44">
         <f>RANK(Table3[[#This Row],[Estimate]],Table3[Estimate])</f>
         <v>8</v>
       </c>
@@ -2775,23 +2898,23 @@
       <c r="A25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="40">
         <v>0</v>
       </c>
       <c r="C25" s="1">
         <v>11</v>
       </c>
-      <c r="D25" s="19">
-        <v>1.0000000000000001E-5</v>
+      <c r="D25" s="40">
+        <v>0</v>
       </c>
       <c r="E25" s="1">
         <v>8</v>
       </c>
       <c r="F25" s="19">
-        <v>3.3369999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>55</v>
@@ -2805,52 +2928,55 @@
       <c r="K25" s="5">
         <v>9</v>
       </c>
-      <c r="M25" s="32" t="s">
+      <c r="M25" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="N25" s="32">
-        <v>154303.99083</v>
-      </c>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32">
-        <v>55719.08</v>
-      </c>
-      <c r="Q25" s="32" t="s">
+      <c r="N25" s="26">
+        <v>4629119.7248999998</v>
+      </c>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26">
+        <v>69842.09</v>
+      </c>
+      <c r="Q25" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="R25" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="32" t="s">
+      <c r="R25" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="V25" s="32">
-        <v>325052.75475999998</v>
-      </c>
+      <c r="V25" s="26">
+        <v>9751582.6428999994</v>
+      </c>
+      <c r="Y25"/>
+      <c r="Z25" s="45"/>
+      <c r="AA25" s="45"/>
     </row>
     <row r="26" spans="1:27" ht="17">
       <c r="A26" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="41">
         <v>0</v>
       </c>
       <c r="C26" s="3">
         <v>6</v>
       </c>
-      <c r="D26" s="20">
-        <v>1.0000000000000001E-5</v>
+      <c r="D26" s="42">
+        <v>0</v>
       </c>
       <c r="E26" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" s="20">
-        <v>9.5E-4</v>
+        <v>0</v>
       </c>
       <c r="G26" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>55</v>
@@ -2859,35 +2985,38 @@
         <v>55</v>
       </c>
       <c r="J26" s="20">
-        <v>1.201E-2</v>
+        <v>0</v>
       </c>
       <c r="K26" s="6">
         <v>19</v>
       </c>
-      <c r="M26" s="32" t="s">
+      <c r="M26" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="N26" s="32">
-        <v>325052.75475999998</v>
-      </c>
-      <c r="O26" s="32"/>
-      <c r="P26" s="32">
-        <v>53191.57</v>
-      </c>
-      <c r="Q26" s="32">
-        <v>6.11</v>
-      </c>
-      <c r="R26" s="33" t="s">
+      <c r="N26" s="26">
+        <v>9751582.6428999994</v>
+      </c>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26">
+        <v>66673.94</v>
+      </c>
+      <c r="Q26" s="26">
+        <v>17.64</v>
+      </c>
+      <c r="R26" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S26" s="33"/>
-      <c r="T26" s="33"/>
-      <c r="U26" s="32" t="s">
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="V26" s="32">
-        <v>299782.36228</v>
-      </c>
+      <c r="V26" s="26">
+        <v>8993470.8683000002</v>
+      </c>
+      <c r="Y26"/>
+      <c r="Z26" s="45"/>
+      <c r="AA26" s="45"/>
     </row>
     <row r="27" spans="1:27" ht="17">
       <c r="A27" s="9" t="s">
@@ -2899,26 +3028,26 @@
       <c r="F27" s="19"/>
       <c r="J27" s="4"/>
       <c r="K27" s="16"/>
-      <c r="M27" s="32" t="s">
+      <c r="M27" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="N27" s="32">
-        <v>299782.36228</v>
-      </c>
-      <c r="O27" s="32"/>
-      <c r="P27" s="32">
-        <v>51814.6</v>
-      </c>
-      <c r="Q27" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="R27" s="33" t="s">
+      <c r="N27" s="26">
+        <v>8993470.8683000002</v>
+      </c>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26">
+        <v>64947.95</v>
+      </c>
+      <c r="Q27" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="R27" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="32"/>
-      <c r="V27" s="32"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="26"/>
       <c r="Y27"/>
     </row>
     <row r="28" spans="1:27" ht="17">
@@ -2926,7 +3055,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="19">
-        <v>2.094E-2</v>
+        <v>0</v>
       </c>
       <c r="C28" s="1">
         <v>18</v>
@@ -2955,14 +3084,16 @@
       <c r="K28" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S28" s="33"/>
-      <c r="T28" s="33"/>
-      <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="V28" s="26"/>
       <c r="Y28"/>
     </row>
     <row r="29" spans="1:27" ht="17">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="19">
@@ -2995,10 +3126,12 @@
       <c r="K29" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S29" s="32"/>
-      <c r="T29" s="32"/>
-      <c r="U29" s="32"/>
-      <c r="V29" s="32"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="V29" s="26"/>
       <c r="Y29"/>
     </row>
     <row r="30" spans="1:27" ht="17">
@@ -3006,19 +3139,19 @@
         <v>32</v>
       </c>
       <c r="B30" s="19">
-        <v>7.9159999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1">
         <v>21</v>
       </c>
       <c r="D30" s="19">
-        <v>0.81235000000000002</v>
+        <v>0.57952000000000004</v>
       </c>
       <c r="E30" s="1">
         <v>23</v>
       </c>
       <c r="F30" s="19">
-        <v>9.0000000000000006E-5</v>
+        <v>0</v>
       </c>
       <c r="G30" s="1">
         <v>10</v>
@@ -3035,10 +3168,20 @@
       <c r="K30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S30" s="34"/>
-      <c r="T30" s="34"/>
-      <c r="U30" s="32"/>
-      <c r="V30" s="32"/>
+      <c r="M30" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="S30" s="28"/>
+      <c r="T30" s="28"/>
+      <c r="U30" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="V30" s="26"/>
       <c r="Y30"/>
     </row>
     <row r="31" spans="1:27" ht="17">
@@ -3058,7 +3201,7 @@
         <v>6</v>
       </c>
       <c r="F31" s="19">
-        <v>1.1900000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="G31" s="1">
         <v>11</v>
@@ -3075,10 +3218,20 @@
       <c r="K31" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S31" s="34"/>
-      <c r="T31" s="34"/>
-      <c r="U31" s="32"/>
-      <c r="V31" s="32"/>
+      <c r="M31" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="26">
+        <v>0</v>
+      </c>
+      <c r="S31" s="28"/>
+      <c r="T31" s="28"/>
+      <c r="U31" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="V31" s="26"/>
       <c r="Y31"/>
     </row>
     <row r="32" spans="1:27" ht="17">
@@ -3086,19 +3239,19 @@
         <v>34</v>
       </c>
       <c r="B32" s="19">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="C32" s="1">
         <v>10</v>
       </c>
       <c r="D32" s="19">
-        <v>1.6979999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1">
         <v>18</v>
       </c>
       <c r="F32" s="19">
-        <v>0.44746000000000002</v>
+        <v>1.47E-3</v>
       </c>
       <c r="G32" s="1">
         <v>19</v>
@@ -3115,10 +3268,20 @@
       <c r="K32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S32" s="32"/>
-      <c r="T32" s="32"/>
-      <c r="U32" s="32"/>
-      <c r="V32" s="32"/>
+      <c r="M32" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26">
+        <v>0</v>
+      </c>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="V32" s="26"/>
       <c r="Y32"/>
     </row>
     <row r="33" spans="1:25" ht="17">
@@ -3126,7 +3289,7 @@
         <v>35</v>
       </c>
       <c r="B33" s="19">
-        <v>6.0000000000000002E-5</v>
+        <v>0</v>
       </c>
       <c r="C33" s="1">
         <v>12</v>
@@ -3138,7 +3301,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="19">
-        <v>0.11062</v>
+        <v>0</v>
       </c>
       <c r="G33" s="1">
         <v>17</v>
@@ -3155,10 +3318,20 @@
       <c r="K33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S33" s="33"/>
-      <c r="T33" s="33"/>
-      <c r="U33" s="32"/>
-      <c r="V33" s="32"/>
+      <c r="M33" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26">
+        <v>0</v>
+      </c>
+      <c r="S33" s="27"/>
+      <c r="T33" s="27"/>
+      <c r="U33" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="V33" s="26"/>
       <c r="Y33"/>
     </row>
     <row r="34" spans="1:25" ht="17">
@@ -3172,13 +3345,13 @@
         <v>8</v>
       </c>
       <c r="D34" s="19">
-        <v>0.56942999999999999</v>
+        <v>0.15039</v>
       </c>
       <c r="E34" s="1">
         <v>21</v>
       </c>
       <c r="F34" s="19">
-        <v>6.9999999999999994E-5</v>
+        <v>0</v>
       </c>
       <c r="G34" s="1">
         <v>9</v>
@@ -3195,10 +3368,20 @@
       <c r="K34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S34" s="32"/>
-      <c r="T34" s="32"/>
-      <c r="U34" s="32"/>
-      <c r="V34" s="32"/>
+      <c r="M34" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26">
+        <v>0</v>
+      </c>
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="V34" s="26"/>
       <c r="Y34"/>
     </row>
     <row r="35" spans="1:25" ht="17">
@@ -3235,10 +3418,20 @@
       <c r="K35" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S35" s="33"/>
-      <c r="T35" s="33"/>
-      <c r="U35" s="32"/>
-      <c r="V35" s="32"/>
+      <c r="M35" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26">
+        <v>0</v>
+      </c>
+      <c r="S35" s="27"/>
+      <c r="T35" s="27"/>
+      <c r="U35" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="V35" s="26"/>
       <c r="Y35"/>
     </row>
     <row r="36" spans="1:25" ht="17">
@@ -3246,13 +3439,13 @@
         <v>38</v>
       </c>
       <c r="B36" s="19">
-        <v>4.9300000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="C36" s="1">
         <v>14</v>
       </c>
       <c r="D36" s="19">
-        <v>0.58255999999999997</v>
+        <v>0.65529000000000004</v>
       </c>
       <c r="E36" s="1">
         <v>22</v>
@@ -3275,10 +3468,20 @@
       <c r="K36" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S36" s="32"/>
-      <c r="T36" s="32"/>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
+      <c r="M36" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26">
+        <v>0</v>
+      </c>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="V36" s="26"/>
       <c r="Y36"/>
     </row>
     <row r="37" spans="1:25" ht="17">
@@ -3286,19 +3489,19 @@
         <v>39</v>
       </c>
       <c r="B37" s="19">
-        <v>9.0000000000000006E-5</v>
+        <v>0</v>
       </c>
       <c r="C37" s="1">
         <v>13</v>
       </c>
       <c r="D37" s="19">
-        <v>6.1700000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="E37" s="1">
         <v>17</v>
       </c>
       <c r="F37" s="19">
-        <v>0.44174999999999998</v>
+        <v>1.2800000000000001E-3</v>
       </c>
       <c r="G37" s="1">
         <v>20</v>
@@ -3315,10 +3518,20 @@
       <c r="K37" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S37" s="32"/>
-      <c r="T37" s="32"/>
-      <c r="U37" s="32"/>
-      <c r="V37" s="32"/>
+      <c r="M37" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26">
+        <v>0</v>
+      </c>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="V37" s="26"/>
       <c r="Y37"/>
     </row>
     <row r="38" spans="1:25" ht="17">
@@ -3326,19 +3539,19 @@
         <v>40</v>
       </c>
       <c r="B38" s="19">
-        <v>3.0589999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="C38" s="1">
         <v>20</v>
       </c>
       <c r="D38" s="19">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
         <v>13</v>
       </c>
       <c r="F38" s="19">
-        <v>0.68186999999999998</v>
+        <v>8.6099999999999996E-2</v>
       </c>
       <c r="G38" s="1">
         <v>22</v>
@@ -3355,29 +3568,39 @@
       <c r="K38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S38" s="33"/>
-      <c r="T38" s="33"/>
-      <c r="U38" s="32"/>
-      <c r="V38" s="32"/>
+      <c r="M38" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26">
+        <v>0</v>
+      </c>
+      <c r="S38" s="27"/>
+      <c r="T38" s="27"/>
+      <c r="U38" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="V38" s="26"/>
     </row>
     <row r="39" spans="1:25" ht="17">
       <c r="A39" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B39" s="19">
-        <v>2.6159999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="C39" s="1">
         <v>16</v>
       </c>
       <c r="D39" s="19">
-        <v>2.24E-2</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1">
         <v>15</v>
       </c>
       <c r="F39" s="19">
-        <v>4.0750000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G39" s="1">
         <v>15</v>
@@ -3394,17 +3617,27 @@
       <c r="K39" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S39" s="32"/>
-      <c r="T39" s="32"/>
-      <c r="U39" s="32"/>
-      <c r="V39" s="32"/>
+      <c r="M39" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26">
+        <v>0</v>
+      </c>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="V39" s="26"/>
     </row>
     <row r="40" spans="1:25" ht="17">
       <c r="A40" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B40" s="19">
-        <v>0.57647999999999999</v>
+        <v>2.623E-2</v>
       </c>
       <c r="C40" s="1">
         <v>23</v>
@@ -3416,7 +3649,7 @@
         <v>7</v>
       </c>
       <c r="F40" s="19">
-        <v>0.75158999999999998</v>
+        <v>0.18501999999999999</v>
       </c>
       <c r="G40" s="1">
         <v>23</v>
@@ -3433,17 +3666,27 @@
       <c r="K40" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S40" s="34"/>
-      <c r="T40" s="34"/>
-      <c r="U40" s="32"/>
-      <c r="V40" s="32"/>
+      <c r="M40" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26">
+        <v>0</v>
+      </c>
+      <c r="S40" s="28"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="V40" s="26"/>
     </row>
     <row r="41" spans="1:25" ht="17">
       <c r="A41" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B41" s="19">
-        <v>0.36878</v>
+        <v>3.5E-4</v>
       </c>
       <c r="C41" s="1">
         <v>22</v>
@@ -3455,7 +3698,7 @@
         <v>9</v>
       </c>
       <c r="F41" s="19">
-        <v>2.0899999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="G41" s="1">
         <v>13</v>
@@ -3472,29 +3715,39 @@
       <c r="K41" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S41" s="33"/>
-      <c r="T41" s="33"/>
-      <c r="U41" s="32"/>
-      <c r="V41" s="32"/>
+      <c r="M41" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26">
+        <v>0</v>
+      </c>
+      <c r="S41" s="27"/>
+      <c r="T41" s="27"/>
+      <c r="U41" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="V41" s="26"/>
     </row>
     <row r="42" spans="1:25" ht="17">
       <c r="A42" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B42" s="19">
-        <v>3.2809999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="C42" s="1">
         <v>19</v>
       </c>
       <c r="D42" s="19">
-        <v>5.1069999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="E42" s="1">
         <v>19</v>
       </c>
       <c r="F42" s="19">
-        <v>0.4995</v>
+        <v>4.7000000000000002E-3</v>
       </c>
       <c r="G42" s="1">
         <v>21</v>
@@ -3511,29 +3764,39 @@
       <c r="K42" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S42" s="33"/>
-      <c r="T42" s="33"/>
-      <c r="U42" s="32"/>
-      <c r="V42" s="32"/>
+      <c r="M42" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="N42" s="26"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26">
+        <v>0</v>
+      </c>
+      <c r="S42" s="27"/>
+      <c r="T42" s="27"/>
+      <c r="U42" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="V42" s="26"/>
     </row>
     <row r="43" spans="1:25" ht="17">
       <c r="A43" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B43" s="19">
-        <v>8.8900000000000003E-3</v>
+        <v>0</v>
       </c>
       <c r="C43" s="1">
         <v>17</v>
       </c>
       <c r="D43" s="19">
-        <v>1.2999999999999999E-4</v>
+        <v>0</v>
       </c>
       <c r="E43" s="1">
         <v>14</v>
       </c>
       <c r="F43" s="19">
-        <v>0.13435</v>
+        <v>0</v>
       </c>
       <c r="G43" s="1">
         <v>18</v>
@@ -3550,10 +3813,20 @@
       <c r="K43" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S43" s="33"/>
-      <c r="T43" s="33"/>
-      <c r="U43" s="32"/>
-      <c r="V43" s="32"/>
+      <c r="M43" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26">
+        <v>0</v>
+      </c>
+      <c r="S43" s="27"/>
+      <c r="T43" s="27"/>
+      <c r="U43" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="26"/>
     </row>
     <row r="44" spans="1:25" ht="17">
       <c r="A44" s="10" t="s">
@@ -3589,17 +3862,27 @@
       <c r="K44" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S44" s="33"/>
-      <c r="T44" s="33"/>
-      <c r="U44" s="32"/>
-      <c r="V44" s="32"/>
+      <c r="M44" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="N44" s="26"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26">
+        <v>0</v>
+      </c>
+      <c r="S44" s="27"/>
+      <c r="T44" s="27"/>
+      <c r="U44" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="V44" s="26"/>
     </row>
     <row r="45" spans="1:25" ht="17">
       <c r="A45" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B45" s="19">
-        <v>2.4299999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="C45" s="1">
         <v>15</v>
@@ -3611,7 +3894,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="19">
-        <v>1.01E-3</v>
+        <v>0</v>
       </c>
       <c r="G45" s="1">
         <v>12</v>
@@ -3628,10 +3911,22 @@
       <c r="K45" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S45" s="32"/>
-      <c r="T45" s="32"/>
-    </row>
-    <row r="46" spans="1:25">
+      <c r="M45" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="N45" s="26"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="26">
+        <v>0</v>
+      </c>
+      <c r="S45" s="26"/>
+      <c r="T45" s="26"/>
+      <c r="U45" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="V45" s="30"/>
+    </row>
+    <row r="46" spans="1:25" ht="17">
       <c r="A46" s="10" t="s">
         <v>48</v>
       </c>
@@ -3648,7 +3943,7 @@
         <v>10</v>
       </c>
       <c r="F46" s="19">
-        <v>3.7080000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="G46" s="1">
         <v>16</v>
@@ -3665,8 +3960,19 @@
       <c r="K46" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:25">
+      <c r="M46" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="N46" s="26"/>
+      <c r="O46" s="26"/>
+      <c r="P46" s="26">
+        <v>0</v>
+      </c>
+      <c r="U46" s="37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="17">
       <c r="A47" s="11" t="s">
         <v>49</v>
       </c>
@@ -3677,13 +3983,13 @@
         <v>6</v>
       </c>
       <c r="D47" s="19">
-        <v>6.2399999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="E47" s="1">
         <v>16</v>
       </c>
       <c r="F47" s="19">
-        <v>5.6299999999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="G47" s="1">
         <v>14</v>
@@ -3700,8 +4006,19 @@
       <c r="K47" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="48" spans="1:25">
+      <c r="M47" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="N47" s="26"/>
+      <c r="O47" s="26"/>
+      <c r="P47" s="26">
+        <v>0</v>
+      </c>
+      <c r="U47" s="38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" ht="17">
       <c r="A48" s="8" t="s">
         <v>50</v>
       </c>
@@ -3735,13 +4052,24 @@
       <c r="K48" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="M48" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="N48" s="26"/>
+      <c r="O48" s="26"/>
+      <c r="P48" s="26">
+        <v>0</v>
+      </c>
+      <c r="U48" s="37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="17">
       <c r="A49" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="19">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="C49" s="1">
         <v>11</v>
@@ -3770,8 +4098,19 @@
       <c r="K49" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="M49" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
+      <c r="P49" s="26">
+        <v>0</v>
+      </c>
+      <c r="U49" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="17">
       <c r="A50" s="13" t="s">
         <v>52</v>
       </c>
@@ -3782,7 +4121,7 @@
         <v>5</v>
       </c>
       <c r="D50" s="20">
-        <v>0.49086000000000002</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E50" s="3">
         <v>20</v>
@@ -3805,8 +4144,19 @@
       <c r="K50" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="M50" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="N50" s="26"/>
+      <c r="O50" s="26"/>
+      <c r="P50" s="26">
+        <v>0</v>
+      </c>
+      <c r="U50" s="37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="17">
       <c r="A51" s="24" t="s">
         <v>56</v>
       </c>
@@ -3820,25 +4170,34 @@
       <c r="I51" s="23"/>
       <c r="J51" s="23"/>
       <c r="K51" s="16"/>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="25" t="s">
+      <c r="M51" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
+      <c r="P51" s="26">
+        <v>0</v>
+      </c>
+      <c r="U51"/>
+    </row>
+    <row r="52" spans="1:21" ht="17">
+      <c r="A52" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="20">
-        <v>0.16064000000000001</v>
+      <c r="B52" s="46">
+        <v>0</v>
       </c>
       <c r="C52" s="3">
         <v>1</v>
       </c>
-      <c r="D52" s="20">
-        <v>0.72821000000000002</v>
+      <c r="D52" s="46">
+        <v>0</v>
       </c>
       <c r="E52" s="3">
         <v>1</v>
       </c>
-      <c r="F52" s="20">
-        <v>0.43157000000000001</v>
+      <c r="F52" s="46">
+        <v>0.02</v>
       </c>
       <c r="G52" s="3">
         <v>1</v>
@@ -3849,16 +4208,21 @@
       <c r="I52" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J52" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K52" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M52"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="M53"/>
+      <c r="J52" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K52" s="6">
+        <v>1</v>
+      </c>
+      <c r="M52" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
+      <c r="P52" s="26">
+        <v>0</v>
+      </c>
+      <c r="U52"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3871,17 +4235,22 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E26 B28:E50">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="C5:C26 B28:E50 E5:E26">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:G26 B28:G50">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+  <conditionalFormatting sqref="C5:C26 B28:G50 E5:G26">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J26">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B26">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>

</xml_diff>